<commit_message>
Add feedback to intial results
</commit_message>
<xml_diff>
--- a/GPAvFeedbackRegression.xlsx
+++ b/GPAvFeedbackRegression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b75b1c6a55d49cb/College/JuniorYear/CS5140/Grade Data Mining Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3BF53630-E0A2-41CC-B40D-A50DD202B31A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{229FFD84-488A-4EB2-9439-3B7AF4EBCC93}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{3BF53630-E0A2-41CC-B40D-A50DD202B31A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{63A512B8-B9DE-4ED5-852E-18684831B20F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7290" windowWidth="24900" windowHeight="11700" xr2:uid="{63CB9C1A-D7D1-4115-9934-05DE03ACB8DD}"/>
+    <workbookView xWindow="43590" yWindow="2505" windowWidth="26100" windowHeight="16545" xr2:uid="{63CB9C1A-D7D1-4115-9934-05DE03ACB8DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,28 +189,50 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1736524200850439E-4"/>
+                  <c:y val="-0.14293692669859567"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>3.23041474654377</c:v>
                 </c:pt>
@@ -309,10 +331,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>3.9020618556700999</c:v>
                 </c:pt>
@@ -412,7 +434,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F694-4EBC-B68D-EE9FF8E38C72}"/>
+              <c16:uniqueId val="{00000000-527B-4CFB-9751-49670328489B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -424,13 +446,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="724142872"/>
-        <c:axId val="724143200"/>
+        <c:axId val="831076680"/>
+        <c:axId val="831073400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="724142872"/>
+        <c:axId val="831076680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -449,7 +472,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -485,14 +508,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="724143200"/>
+        <c:crossAx val="831073400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="724143200"/>
+        <c:axId val="831073400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -511,7 +535,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -547,7 +571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="724142872"/>
+        <c:crossAx val="831076680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -559,6 +583,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1163,23 +1218,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42596F92-224A-4179-BBC6-3147CCC9EDB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8490F7C-460A-426E-8D3C-8D226E60CE07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1499,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9165D7CC-90A7-4E27-823D-120F872CBDF8}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>